<commit_message>
Commited by Asif on 01/01/2021
</commit_message>
<xml_diff>
--- a/Fintoo/Data/data_sheet.xlsx
+++ b/Fintoo/Data/data_sheet.xlsx
@@ -1,47 +1,146 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Form" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>User_EmailMob</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>asif.inamdar@fintoo.in</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>asi.inamdar45@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>CNIC #</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>License Type</t>
+  </si>
+  <si>
+    <t>Phone / Whatsapp #</t>
+  </si>
+  <si>
+    <t>Apointment Status</t>
+  </si>
+  <si>
+    <t>Learners Driving License</t>
+  </si>
+  <si>
+    <t>03333612663</t>
+  </si>
+  <si>
+    <t>Nazimabad</t>
+  </si>
+  <si>
+    <t>Permemant Driving License (Commercial)</t>
+  </si>
+  <si>
+    <t>Korangi</t>
+  </si>
+  <si>
+    <t>International Driving Permit (IDP)</t>
+  </si>
+  <si>
+    <t>RHQ Hyderabad</t>
+  </si>
+  <si>
+    <t>TokenNo</t>
+  </si>
+  <si>
+    <t>BookingDate</t>
+  </si>
+  <si>
+    <t>DealTime</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>2021-04-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>BADIN</t>
+  </si>
+  <si>
+    <t>ProvideTimeSlot</t>
+  </si>
+  <si>
+    <t>RequiredTimeSlot</t>
+  </si>
+  <si>
+    <t>10-11</t>
+  </si>
+  <si>
+    <t>10:36</t>
+  </si>
+  <si>
+    <t>9-10</t>
+  </si>
+  <si>
+    <t>Asad shah</t>
+  </si>
+  <si>
+    <t>Saif ahmed</t>
+  </si>
+  <si>
+    <t>Sayed shah</t>
+  </si>
+  <si>
+    <t>abdullah</t>
+  </si>
+  <si>
+    <t>14255-1455728-8</t>
+  </si>
+  <si>
+    <t>14256-1455224-9</t>
+  </si>
+  <si>
+    <t>14256-1455524-1</t>
+  </si>
+  <si>
+    <t>14256-1455534-1</t>
+  </si>
+  <si>
+    <t>15-16</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>484</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
+    <t>09:30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,20 +149,36 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,17 +190,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -144,7 +260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,7 +295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,63 +504,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="36" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>9604768039</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3333612663</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>9604768039</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3333612663</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3333612663</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1" display="asif.inamdar@fintoo.in"/>
     <hyperlink ref="A4" r:id="rId2" display="asif.inamdar@fintoo.in"/>
-    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId3" display="asi.inamdar45@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>